<commit_message>
Update to hours worked from Spencer
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Sawyer</t>
   </si>
@@ -36,6 +36,33 @@
   </si>
   <si>
     <t>Hours Worked</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Sun - 07/15</t>
+  </si>
+  <si>
+    <t>Mon - 07/16</t>
+  </si>
+  <si>
+    <t>Tue - 07/17</t>
+  </si>
+  <si>
+    <t>Wed - 07/18</t>
+  </si>
+  <si>
+    <t>Thu - 07/19</t>
+  </si>
+  <si>
+    <t>Fri - 07/20</t>
+  </si>
+  <si>
+    <t>Sat - 07/21</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -59,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -67,12 +94,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,33 +399,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="2">
+        <f>SUM(C3:I3)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="2">
+        <f>SUM(C4:I4)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="2">
+        <f>SUM(C5:I5)</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to hours worked
spencer added hours
</commit_message>
<xml_diff>
--- a/Hours Worked.xlsx
+++ b/Hours Worked.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" s="2">
         <f>SUM(C5:I5)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -503,7 +503,9 @@
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>4</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>

</xml_diff>